<commit_message>
Ready to run again, a few times
</commit_message>
<xml_diff>
--- a/Baseline-experimental-results.xlsx
+++ b/Baseline-experimental-results.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="Blad2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
   <si>
     <t>Dataset</t>
   </si>
@@ -61,11 +62,29 @@
   <si>
     <t>20 epochs</t>
   </si>
+  <si>
+    <t>128_bin</t>
+  </si>
+  <si>
+    <t>128_bin_times_10</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>std.dev</t>
+  </si>
+  <si>
+    <t>std.err</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.000000%"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -103,11 +122,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Procent" xfId="1" builtinId="5"/>
@@ -140,7 +160,37 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -230,41 +280,38 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Blad1!$A$10:$A$13</c:f>
+              <c:f>Blad1!$A$10:$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>128_over_99</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>128_over_9</c:v>
+                  <c:v>128_times_10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>128</c:v>
+                  <c:v>128_bin</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>128_times_10</c:v>
+                  <c:v>128_bin_times_10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Blad1!$B$10:$B$13</c:f>
+              <c:f>Blad1!$B$10:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.94940000000000002</c:v>
+                  <c:v>0.89810000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.91390000000000005</c:v>
+                  <c:v>0.98240000000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.89810000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.98240000000000005</c:v>
+                  <c:v>0.9012</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -358,41 +405,32 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Blad1!$A$10:$A$13</c:f>
+              <c:f>Blad1!$A$10:$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>128_over_99</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>128_over_9</c:v>
+                  <c:v>128_times_10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>128</c:v>
+                  <c:v>128_bin</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>128_times_10</c:v>
+                  <c:v>128_bin_times_10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Blad1!$C$10:$C$13</c:f>
+              <c:f>Blad1!$C$10:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.96279999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.90849999999999997</c:v>
-                </c:pt>
-                <c:pt idx="2">
                   <c:v>0.90549999999999997</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -475,6 +513,20 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -586,7 +638,687 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="nl-NL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>10-Fold</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Cross-Validation Accuracy</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad2!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>128_over_99</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="nl-NL"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Blad2!$B$14</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>1.5383761461398532E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Blad2!$B$14</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>1.5383761461398532E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Blad2!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>128_over_99</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128_bin</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad2!$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.95515222300000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FF14-4A54-9198-0EEDD51A56AA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="75"/>
+        <c:overlap val="40"/>
+        <c:axId val="478668144"/>
+        <c:axId val="478674704"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent2"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="75000"/>
+                              <a:lumOff val="25000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="nl-NL"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="outEnd"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:round/>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Blad2!$B$1:$D$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>128_over_99</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>128_bin</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Blad2!$C$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-FF14-4A54-9198-0EEDD51A56AA}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent3"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="75000"/>
+                              <a:lumOff val="25000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="nl-NL"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="outEnd"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:round/>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Blad2!$B$1:$D$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>128_over_99</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>128_bin</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Blad2!$D$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="1"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-FF14-4A54-9198-0EEDD51A56AA}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="478668144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="478674704"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="478674704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0.8"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="478668144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1129,20 +1861,523 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>623886</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>104774</xdr:rowOff>
+      <xdr:colOff>642936</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1150,6 +2385,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F3A9D47-8B0A-4849-B962-BE29EF1D4A76}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>366712</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>61912</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafiek 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A543E454-DF1F-4A63-B631-44C193505D07}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1467,19 +2743,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="10" width="12.85546875" customWidth="1"/>
+    <col min="2" max="13" width="17" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1507,8 +2784,20 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1533,8 +2822,14 @@
       <c r="H2">
         <v>196540</v>
       </c>
+      <c r="J2">
+        <v>21620</v>
+      </c>
+      <c r="K2">
+        <v>21620</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1559,8 +2854,14 @@
       <c r="H3">
         <v>49135</v>
       </c>
+      <c r="J3">
+        <v>5405</v>
+      </c>
+      <c r="K3">
+        <v>5405</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1585,8 +2886,14 @@
       <c r="H4">
         <v>621</v>
       </c>
+      <c r="J4">
+        <v>621</v>
+      </c>
+      <c r="K4">
+        <v>621</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1611,8 +2918,14 @@
       <c r="H5">
         <v>10</v>
       </c>
+      <c r="J5">
+        <v>10</v>
+      </c>
+      <c r="K5">
+        <v>10</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1638,8 +2951,11 @@
         <v>1.7600000000000001E-2</v>
       </c>
       <c r="I6" s="1"/>
+      <c r="J6" s="1">
+        <v>9.8800000000000013E-2</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1648,7 +2964,7 @@
         <v>0.94940000000000002</v>
       </c>
       <c r="C7" s="2">
-        <f t="shared" ref="C7:H7" si="0">1-C6</f>
+        <f t="shared" ref="C7:M7" si="0">1-C6</f>
         <v>0.96279999999999999</v>
       </c>
       <c r="D7" s="2">
@@ -1671,9 +2987,28 @@
         <f t="shared" si="0"/>
         <v>0.98240000000000005</v>
       </c>
-      <c r="I7" s="2"/>
+      <c r="I7" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.9012</v>
+      </c>
+      <c r="K7" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L7" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>10</v>
       </c>
@@ -1681,7 +3016,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
@@ -1694,7 +3029,7 @@
         <v>0.96279999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
@@ -1707,7 +3042,7 @@
         <v>0.90849999999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>128</v>
       </c>
@@ -1720,7 +3055,7 @@
         <v>0.90549999999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
@@ -1728,9 +3063,167 @@
         <f>H7</f>
         <v>0.98240000000000005</v>
       </c>
-      <c r="C13" s="2">
-        <f>I7</f>
-        <v>0</v>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2">
+        <f>J7</f>
+        <v>0.9012</v>
+      </c>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.95257610999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0.95960188000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.96135831000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.95081967000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.95199062999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.95140515000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.94847775000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.96077283000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.95257610999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0.96194378999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1">
+        <f>AVERAGE(B2:B11)</f>
+        <v>0.95515222300000002</v>
+      </c>
+      <c r="C12" t="e">
+        <f>AVERAGE(C2:C11)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <f>_xlfn.STDEV.P(B2:B11)</f>
+        <v>4.864772519873984E-3</v>
+      </c>
+      <c r="C13" t="e">
+        <f>_xlfn.STDEV.P(C2:C11)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <f>B13/SQRT(10)</f>
+        <v>1.5383761461398532E-3</v>
+      </c>
+      <c r="C14" t="e">
+        <f>C13/SQRT(10)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed Original folder and Chinese-font folders
</commit_message>
<xml_diff>
--- a/Baseline-experimental-results.xlsx
+++ b/Baseline-experimental-results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
   <si>
     <t>Dataset</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>std.err</t>
+  </si>
+  <si>
+    <t>128_time_10</t>
   </si>
 </sst>
 </file>
@@ -776,7 +779,7 @@
                 <a:endParaRPr lang="nl-NL"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="inEnd"/>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -848,26 +851,38 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Blad2!$B$1:$D$1</c:f>
+              <c:f>Blad2!$B$1:$F$1</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>128_over_99</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>128_bin</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128_time_10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128_bin_times_10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Blad2!$B$12</c:f>
+              <c:f>Blad2!$B$12:$F$12</c:f>
               <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0" formatCode="0.00%">
                   <c:v>0.95515222300000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -875,6 +890,229 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-FF14-4A54-9198-0EEDD51A56AA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="nl-NL"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Blad2!$B$1:$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>128_over_99</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128_bin</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128_time_10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128_bin_times_10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad2!$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FF14-4A54-9198-0EEDD51A56AA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="nl-NL"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Blad2!$B$1:$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>128_over_99</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128_bin</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128_time_10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128_bin_times_10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad2!$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FF14-4A54-9198-0EEDD51A56AA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -891,241 +1129,7 @@
         <c:overlap val="40"/>
         <c:axId val="478668144"/>
         <c:axId val="478674704"/>
-        <c:extLst>
-          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-            <c15:filteredBarSeries>
-              <c15:ser>
-                <c:idx val="1"/>
-                <c:order val="1"/>
-                <c:spPr>
-                  <a:solidFill>
-                    <a:schemeClr val="accent2"/>
-                  </a:solidFill>
-                  <a:ln>
-                    <a:noFill/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:invertIfNegative val="0"/>
-                <c:dLbls>
-                  <c:spPr>
-                    <a:noFill/>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                  <c:txPr>
-                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                      <a:spAutoFit/>
-                    </a:bodyPr>
-                    <a:lstStyle/>
-                    <a:p>
-                      <a:pPr>
-                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                          <a:solidFill>
-                            <a:schemeClr val="tx1">
-                              <a:lumMod val="75000"/>
-                              <a:lumOff val="25000"/>
-                            </a:schemeClr>
-                          </a:solidFill>
-                          <a:latin typeface="+mn-lt"/>
-                          <a:ea typeface="+mn-ea"/>
-                          <a:cs typeface="+mn-cs"/>
-                        </a:defRPr>
-                      </a:pPr>
-                      <a:endParaRPr lang="nl-NL"/>
-                    </a:p>
-                  </c:txPr>
-                  <c:dLblPos val="outEnd"/>
-                  <c:showLegendKey val="0"/>
-                  <c:showVal val="1"/>
-                  <c:showCatName val="0"/>
-                  <c:showSerName val="0"/>
-                  <c:showPercent val="0"/>
-                  <c:showBubbleSize val="0"/>
-                  <c:showLeaderLines val="0"/>
-                  <c:extLst>
-                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                      <c15:showLeaderLines val="1"/>
-                      <c15:leaderLines>
-                        <c:spPr>
-                          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                            <a:solidFill>
-                              <a:schemeClr val="tx1">
-                                <a:lumMod val="35000"/>
-                                <a:lumOff val="65000"/>
-                              </a:schemeClr>
-                            </a:solidFill>
-                            <a:round/>
-                          </a:ln>
-                          <a:effectLst/>
-                        </c:spPr>
-                      </c15:leaderLines>
-                    </c:ext>
-                  </c:extLst>
-                </c:dLbls>
-                <c:cat>
-                  <c:strRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Blad2!$B$1:$D$1</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="2"/>
-                      <c:pt idx="0">
-                        <c:v>128_over_99</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>128_bin</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c:cat>
-                <c:val>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Blad2!$C$12</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="1"/>
-                      <c:pt idx="0">
-                        <c:v>0</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:val>
-                <c:extLst>
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000001-FF14-4A54-9198-0EEDD51A56AA}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredBarSeries>
-            <c15:filteredBarSeries>
-              <c15:ser>
-                <c:idx val="2"/>
-                <c:order val="2"/>
-                <c:spPr>
-                  <a:solidFill>
-                    <a:schemeClr val="accent3"/>
-                  </a:solidFill>
-                  <a:ln>
-                    <a:noFill/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:invertIfNegative val="0"/>
-                <c:dLbls>
-                  <c:spPr>
-                    <a:noFill/>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                  <c:txPr>
-                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                      <a:spAutoFit/>
-                    </a:bodyPr>
-                    <a:lstStyle/>
-                    <a:p>
-                      <a:pPr>
-                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                          <a:solidFill>
-                            <a:schemeClr val="tx1">
-                              <a:lumMod val="75000"/>
-                              <a:lumOff val="25000"/>
-                            </a:schemeClr>
-                          </a:solidFill>
-                          <a:latin typeface="+mn-lt"/>
-                          <a:ea typeface="+mn-ea"/>
-                          <a:cs typeface="+mn-cs"/>
-                        </a:defRPr>
-                      </a:pPr>
-                      <a:endParaRPr lang="nl-NL"/>
-                    </a:p>
-                  </c:txPr>
-                  <c:dLblPos val="outEnd"/>
-                  <c:showLegendKey val="0"/>
-                  <c:showVal val="1"/>
-                  <c:showCatName val="0"/>
-                  <c:showSerName val="0"/>
-                  <c:showPercent val="0"/>
-                  <c:showBubbleSize val="0"/>
-                  <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                      <c15:showLeaderLines val="1"/>
-                      <c15:leaderLines>
-                        <c:spPr>
-                          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                            <a:solidFill>
-                              <a:schemeClr val="tx1">
-                                <a:lumMod val="35000"/>
-                                <a:lumOff val="65000"/>
-                              </a:schemeClr>
-                            </a:solidFill>
-                            <a:round/>
-                          </a:ln>
-                          <a:effectLst/>
-                        </c:spPr>
-                      </c15:leaderLines>
-                    </c:ext>
-                  </c:extLst>
-                </c:dLbls>
-                <c:cat>
-                  <c:strRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Blad2!$B$1:$D$1</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="2"/>
-                      <c:pt idx="0">
-                        <c:v>128_over_99</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>128_bin</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c:cat>
-                <c:val>
-                  <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Blad2!$D$12</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="1"/>
-                    </c:numCache>
-                  </c:numRef>
-                </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000002-FF14-4A54-9198-0EEDD51A56AA}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredBarSeries>
-          </c:ext>
-        </c:extLst>
+        <c:extLst/>
       </c:barChart>
       <c:catAx>
         <c:axId val="478668144"/>
@@ -2412,16 +2416,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>366712</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>14287</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>61912</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2748,8 +2752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2925,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="K5">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -3097,26 +3101,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1">
+        <v>128</v>
+      </c>
+      <c r="D1" t="s">
         <v>12</v>
       </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3124,7 +3137,7 @@
         <v>0.95257610999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3132,7 +3145,7 @@
         <v>0.95960188000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3140,7 +3153,7 @@
         <v>0.96135831000000005</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3148,7 +3161,7 @@
         <v>0.95081967000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3156,7 +3169,7 @@
         <v>0.95199062999999995</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3164,7 +3177,7 @@
         <v>0.95140515000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3172,7 +3185,7 @@
         <v>0.94847775000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3180,7 +3193,7 @@
         <v>0.96077283000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3188,7 +3201,7 @@
         <v>0.95257610999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3196,7 +3209,7 @@
         <v>0.96194378999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -3209,7 +3222,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -3222,7 +3235,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
added binary times 10 dataset, named 128_bin_times_10
</commit_message>
<xml_diff>
--- a/Baseline-experimental-results.xlsx
+++ b/Baseline-experimental-results.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
   <si>
     <t>Dataset</t>
   </si>
@@ -77,16 +77,14 @@
   <si>
     <t>std.err</t>
   </si>
-  <si>
-    <t>128_time_10</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000000%"/>
+    <numFmt numFmtId="168" formatCode="0.00000%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -125,12 +123,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Procent" xfId="1" builtinId="5"/>
@@ -683,9 +682,8 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Cross-Validation Accuracy</a:t>
+              <a:t> Cross-Validation Accuracy ( 10 epochs)</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -749,6 +747,20 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:dLbls>
             <c:spPr>
               <a:noFill/>
@@ -813,12 +825,15 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Blad2!$B$14</c:f>
+                <c:f>Blad2!$B$14:$F$14</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="1"/>
+                  <c:ptCount val="5"/>
                   <c:pt idx="0">
                     <c:v>1.5383761461398532E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.007858168867026E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -864,7 +879,7 @@
                   <c:v>128_bin</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>128_time_10</c:v>
+                  <c:v>128_times_10</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>128_bin_times_10</c:v>
@@ -876,13 +891,13 @@
             <c:numRef>
               <c:f>Blad2!$B$12:$F$12</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="0" formatCode="0.00%">
+                <c:pt idx="0">
                   <c:v>0.95515222300000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.96846780000000021</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -894,121 +909,8 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="2"/>
           <c:order val="1"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="nl-NL"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Blad2!$B$1:$F$1</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>128_over_99</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>128_bin</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>128_time_10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>128_bin_times_10</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Blad2!$C$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
-            </c:numRef>
-          </c:val>
-          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-FF14-4A54-9198-0EEDD51A56AA}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent3"/>
@@ -1092,7 +994,7 @@
                   <c:v>128_bin</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>128_time_10</c:v>
+                  <c:v>128_times_10</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>128_bin_times_10</c:v>
@@ -3104,12 +3006,14 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="7" width="12.42578125" customWidth="1"/>
+    <col min="2" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="7" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3123,7 +3027,7 @@
         <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
         <v>13</v>
@@ -3136,6 +3040,12 @@
       <c r="B2" s="4">
         <v>0.95257610999999998</v>
       </c>
+      <c r="C2" s="4">
+        <v>0.97039229999999999</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -3144,6 +3054,9 @@
       <c r="B3" s="4">
         <v>0.95960188000000002</v>
       </c>
+      <c r="C3" s="4">
+        <v>0.97150259000000005</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -3152,6 +3065,9 @@
       <c r="B4" s="4">
         <v>0.96135831000000005</v>
       </c>
+      <c r="C4" s="4">
+        <v>0.96891190999999999</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -3160,6 +3076,9 @@
       <c r="B5" s="4">
         <v>0.95081967000000001</v>
       </c>
+      <c r="C5" s="4">
+        <v>0.97113249999999995</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -3168,6 +3087,9 @@
       <c r="B6" s="4">
         <v>0.95199062999999995</v>
       </c>
+      <c r="C6" s="4">
+        <v>0.97113249000000001</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -3176,6 +3098,9 @@
       <c r="B7" s="4">
         <v>0.95140515000000003</v>
       </c>
+      <c r="C7" s="4">
+        <v>0.96447075999999998</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -3184,6 +3109,9 @@
       <c r="B8" s="4">
         <v>0.94847775000000001</v>
       </c>
+      <c r="C8" s="4">
+        <v>0.96780162000000003</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -3192,6 +3120,9 @@
       <c r="B9" s="4">
         <v>0.96077283000000002</v>
       </c>
+      <c r="C9" s="4">
+        <v>0.97039229999999999</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -3200,6 +3131,9 @@
       <c r="B10" s="4">
         <v>0.95257610999999998</v>
       </c>
+      <c r="C10" s="4">
+        <v>0.96780162999999997</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -3208,6 +3142,9 @@
       <c r="B11" s="4">
         <v>0.96194378999999997</v>
       </c>
+      <c r="C11" s="4">
+        <v>0.96113990000000005</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -3217,9 +3154,9 @@
         <f>AVERAGE(B2:B11)</f>
         <v>0.95515222300000002</v>
       </c>
-      <c r="C12" t="e">
+      <c r="C12" s="1">
         <f>AVERAGE(C2:C11)</f>
-        <v>#DIV/0!</v>
+        <v>0.96846780000000021</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -3230,9 +3167,9 @@
         <f>_xlfn.STDEV.P(B2:B11)</f>
         <v>4.864772519873984E-3</v>
       </c>
-      <c r="C13" t="e">
+      <c r="C13">
         <f>_xlfn.STDEV.P(C2:C11)</f>
-        <v>#DIV/0!</v>
+        <v>3.1871273720264067E-3</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -3243,9 +3180,9 @@
         <f>B13/SQRT(10)</f>
         <v>1.5383761461398532E-3</v>
       </c>
-      <c r="C14" t="e">
+      <c r="C14">
         <f>C13/SQRT(10)</f>
-        <v>#DIV/0!</v>
+        <v>1.007858168867026E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
deleted wrongly annotated files, so model_k_fold 128 has to be done again.
</commit_message>
<xml_diff>
--- a/Baseline-experimental-results.xlsx
+++ b/Baseline-experimental-results.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t>Dataset</t>
   </si>
@@ -77,6 +77,12 @@
   <si>
     <t>std.err</t>
   </si>
+  <si>
+    <t>128_extended</t>
+  </si>
+  <si>
+    <t>128_extended*10</t>
+  </si>
 </sst>
 </file>
 
@@ -84,7 +90,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000000%"/>
-    <numFmt numFmtId="168" formatCode="0.00000%"/>
+    <numFmt numFmtId="165" formatCode="0.00000%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -129,7 +135,7 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Procent" xfId="1" builtinId="5"/>
@@ -748,7 +754,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dPt>
-            <c:idx val="1"/>
+            <c:idx val="0"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -760,6 +766,16 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-D705-4C09-B5E9-1480ED4D0B21}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -828,12 +844,12 @@
                 <c:f>Blad2!$B$14:$F$14</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
+                  <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>1.5383761461398532E-3</c:v>
+                    <c:v>1.007858168867026E-3</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.007858168867026E-3</c:v>
+                    <c:v>1.0120716118418233E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -841,13 +857,6 @@
             <c:minus>
               <c:numRef>
                 <c:f>Blad2!$B$14</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="1"/>
-                  <c:pt idx="0">
-                    <c:v>1.5383761461398532E-3</c:v>
-                  </c:pt>
-                </c:numCache>
               </c:numRef>
             </c:minus>
             <c:spPr>
@@ -868,20 +877,17 @@
             <c:strRef>
               <c:f>Blad2!$B$1:$F$1</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>128_over_99</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>128</c:v>
+                  <c:v>128_bin</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>128_bin</c:v>
+                  <c:v>128_times_10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>128_times_10</c:v>
-                </c:pt>
-                <c:pt idx="4">
                   <c:v>128_bin_times_10</c:v>
                 </c:pt>
               </c:strCache>
@@ -892,12 +898,12 @@
               <c:f>Blad2!$B$12:$F$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.95515222300000002</c:v>
+                  <c:v>0.96846780000000021</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.96846780000000021</c:v>
+                  <c:v>0.96842105299999992</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -905,116 +911,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-FF14-4A54-9198-0EEDD51A56AA}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="nl-NL"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Blad2!$B$1:$F$1</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>128_over_99</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>128_bin</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>128_times_10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>128_bin_times_10</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Blad2!$D$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
-            </c:numRef>
-          </c:val>
-          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-FF14-4A54-9198-0EEDD51A56AA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3003,20 +2899,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="4" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" hidden="1" customWidth="1"/>
+    <col min="3" max="4" width="12.42578125" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" customWidth="1"/>
     <col min="6" max="7" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -3032,8 +2929,14 @@
       <c r="F1" t="s">
         <v>13</v>
       </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3043,11 +2946,13 @@
       <c r="C2" s="4">
         <v>0.97039229999999999</v>
       </c>
-      <c r="D2" s="5"/>
+      <c r="D2" s="5">
+        <v>0.97034841000000005</v>
+      </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3057,8 +2962,11 @@
       <c r="C3" s="4">
         <v>0.97150259000000005</v>
       </c>
+      <c r="D3" s="5">
+        <v>0.96886583000000004</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3068,8 +2976,11 @@
       <c r="C4" s="4">
         <v>0.96891190999999999</v>
       </c>
+      <c r="D4" s="5">
+        <v>0.96738323999999998</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3079,8 +2990,11 @@
       <c r="C5" s="4">
         <v>0.97113249999999995</v>
       </c>
+      <c r="D5" s="5">
+        <v>0.97220163000000004</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3090,8 +3004,11 @@
       <c r="C6" s="4">
         <v>0.97113249000000001</v>
       </c>
+      <c r="D6" s="5">
+        <v>0.96849518000000001</v>
+      </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3101,8 +3018,11 @@
       <c r="C7" s="4">
         <v>0.96447075999999998</v>
       </c>
+      <c r="D7" s="5">
+        <v>0.97405485999999997</v>
+      </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3112,8 +3032,11 @@
       <c r="C8" s="4">
         <v>0.96780162000000003</v>
       </c>
+      <c r="D8" s="5">
+        <v>0.96515938000000001</v>
+      </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3123,8 +3046,11 @@
       <c r="C9" s="4">
         <v>0.97039229999999999</v>
       </c>
+      <c r="D9" s="5">
+        <v>0.96478872999999998</v>
+      </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3134,8 +3060,11 @@
       <c r="C10" s="4">
         <v>0.96780162999999997</v>
       </c>
+      <c r="D10" s="5">
+        <v>0.96960712000000004</v>
+      </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3145,8 +3074,11 @@
       <c r="C11" s="4">
         <v>0.96113990000000005</v>
       </c>
+      <c r="D11" s="5">
+        <v>0.96330614999999997</v>
+      </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -3158,31 +3090,43 @@
         <f>AVERAGE(C2:C11)</f>
         <v>0.96846780000000021</v>
       </c>
+      <c r="D12" s="1">
+        <f>AVERAGE(D2:D11)</f>
+        <v>0.96842105299999992</v>
+      </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="4">
         <f>_xlfn.STDEV.P(B2:B11)</f>
         <v>4.864772519873984E-3</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="4">
         <f>_xlfn.STDEV.P(C2:C11)</f>
         <v>3.1871273720264067E-3</v>
       </c>
+      <c r="D13" s="4">
+        <f>_xlfn.STDEV.P(D2:D11)</f>
+        <v>3.2004514486180012E-3</v>
+      </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="4">
         <f>B13/SQRT(10)</f>
         <v>1.5383761461398532E-3</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="4">
         <f>C13/SQRT(10)</f>
         <v>1.007858168867026E-3</v>
+      </c>
+      <c r="D14" s="4">
+        <f>D13/SQRT(10)</f>
+        <v>1.0120716118418233E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new results and models
</commit_message>
<xml_diff>
--- a/Baseline-experimental-results.xlsx
+++ b/Baseline-experimental-results.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
-    <sheet name="Blad1" sheetId="1" r:id="rId1"/>
-    <sheet name="Blad2" sheetId="2" r:id="rId2"/>
+    <sheet name="new_results" sheetId="3" r:id="rId1"/>
+    <sheet name="10-fold cross validation" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>Dataset</t>
   </si>
@@ -45,9 +45,6 @@
     <t>128_over_99</t>
   </si>
   <si>
-    <t>128_over_9</t>
-  </si>
-  <si>
     <t>128_times_10</t>
   </si>
   <si>
@@ -55,12 +52,6 @@
   </si>
   <si>
     <t>Accuracy</t>
-  </si>
-  <si>
-    <t>10 epochs</t>
-  </si>
-  <si>
-    <t>20 epochs</t>
   </si>
   <si>
     <t>128_bin</t>
@@ -78,10 +69,34 @@
     <t>std.err</t>
   </si>
   <si>
+    <t>Original</t>
+  </si>
+  <si>
+    <t>Original_bin</t>
+  </si>
+  <si>
+    <t>Extended</t>
+  </si>
+  <si>
+    <t>Extended_bin</t>
+  </si>
+  <si>
+    <t>Augmented</t>
+  </si>
+  <si>
+    <t>Bin_augmented</t>
+  </si>
+  <si>
+    <t>Bin_Augmented</t>
+  </si>
+  <si>
     <t>128_extended</t>
   </si>
   <si>
-    <t>128_extended*10</t>
+    <t>128_extended_bin</t>
+  </si>
+  <si>
+    <t>MEMORY ERROR</t>
   </si>
 </sst>
 </file>
@@ -210,11 +225,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Blad1!$B$9</c:f>
+              <c:f>new_results!$B$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>10 epochs</c:v>
+                  <c:v>Accuracy</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -259,6 +274,7 @@
                 <a:endParaRPr lang="nl-NL"/>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -288,171 +304,59 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Blad1!$A$10:$A$15</c:f>
+              <c:f>new_results!$A$10:$A$15</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>128</c:v>
+                  <c:v>Original</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>128_times_10</c:v>
+                  <c:v>Original_bin</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>128_bin</c:v>
+                  <c:v>Augmented</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>128_bin_times_10</c:v>
+                  <c:v>Bin_Augmented</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Extended</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Extended_bin</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Blad1!$B$10:$B$15</c:f>
+              <c:f>new_results!$B$10:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.89810000000000001</c:v>
+                  <c:v>0.96889999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.98240000000000005</c:v>
+                  <c:v>0.96789999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.9012</c:v>
+                  <c:v>0.97640000000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.97699999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-22F6-4453-A476-D00B8B743A6F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Blad1!$C$9</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>20 epochs</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="nl-NL"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Blad1!$A$10:$A$15</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>128_times_10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>128_bin</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>128_bin_times_10</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Blad1!$C$10:$C$15</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0.90549999999999997</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.9042</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-22F6-4453-A476-D00B8B743A6F}"/>
+              <c16:uniqueId val="{00000000-59AE-4932-B23F-6456F083D2FC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
@@ -460,12 +364,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="75"/>
-        <c:axId val="420805688"/>
-        <c:axId val="420805032"/>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="475002800"/>
+        <c:axId val="475003128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="420805688"/>
+        <c:axId val="475002800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -508,7 +413,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="420805032"/>
+        <c:crossAx val="475003128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -516,11 +421,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="420805032"/>
+        <c:axId val="475003128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
-          <c:min val="0.8"/>
+          <c:min val="0.95000000000000007"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -569,7 +474,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="420805688"/>
+        <c:crossAx val="475002800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -581,37 +486,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -688,7 +562,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Cross-Validation Accuracy ( 10 epochs)</a:t>
+              <a:t> Cross-Validation Accuracy</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -734,7 +608,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Blad2!$B$1</c:f>
+              <c:f>'10-fold cross validation'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -766,6 +640,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-30F7-4A55-8ECD-D983111AFC10}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -841,7 +720,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Blad2!$B$14:$F$14</c:f>
+                <c:f>'10-fold cross validation'!$B$14:$F$14</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
@@ -856,7 +735,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Blad2!$B$14</c:f>
+                <c:f>'10-fold cross validation'!$B$14</c:f>
               </c:numRef>
             </c:minus>
             <c:spPr>
@@ -875,30 +754,36 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Blad2!$B$1:$F$1</c:f>
+              <c:f>'10-fold cross validation'!$B$1:$H$1</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>128</c:v>
+                  <c:v>Original</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>128_bin</c:v>
+                  <c:v>Original_bin</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>128_times_10</c:v>
+                  <c:v>Augmented</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>128_bin_times_10</c:v>
+                  <c:v>Bin_augmented</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Extended</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Extended_bin</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Blad2!$B$12:$F$12</c:f>
+              <c:f>'10-fold cross validation'!$B$12:$H$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0.96846780000000021</c:v>
                 </c:pt>
@@ -2173,23 +2058,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>642936</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>376237</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>300037</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Grafiek 2">
+        <xdr:cNvPr id="2" name="Grafiek 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F3A9D47-8B0A-4849-B962-BE29EF1D4A76}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C920186E-20F9-4C71-8A4F-052BC22FCB2C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2548,348 +2433,214 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="13" width="17" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>5</v>
+      <c r="B1">
+        <v>128</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
         <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1">
-        <v>128</v>
-      </c>
-      <c r="G1">
-        <v>128</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>13665</v>
+        <v>21584</v>
       </c>
       <c r="C2">
-        <v>13666</v>
+        <v>21584</v>
       </c>
       <c r="D2">
-        <v>20811</v>
+        <v>196180</v>
       </c>
       <c r="E2">
-        <v>20812</v>
-      </c>
-      <c r="F2">
-        <v>21620</v>
-      </c>
-      <c r="G2">
-        <v>21620</v>
-      </c>
-      <c r="H2">
-        <v>196540</v>
-      </c>
-      <c r="J2">
-        <v>21620</v>
-      </c>
-      <c r="K2">
-        <v>21620</v>
+        <v>196110</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>3417</v>
+        <v>5396</v>
       </c>
       <c r="C3">
-        <v>3416</v>
+        <v>5396</v>
       </c>
       <c r="D3">
-        <v>5203</v>
+        <v>49045</v>
       </c>
       <c r="E3">
-        <v>5202</v>
-      </c>
-      <c r="F3">
-        <v>5405</v>
-      </c>
-      <c r="G3">
-        <v>5405</v>
-      </c>
-      <c r="H3">
-        <v>49135</v>
-      </c>
-      <c r="J3">
-        <v>5405</v>
-      </c>
-      <c r="K3">
-        <v>5405</v>
+        <v>49027</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4">
-        <v>82</v>
+        <v>589</v>
       </c>
       <c r="C4">
-        <v>82</v>
+        <v>589</v>
       </c>
       <c r="D4">
-        <v>360</v>
+        <v>589</v>
       </c>
       <c r="E4">
-        <v>360</v>
-      </c>
-      <c r="F4">
-        <v>621</v>
-      </c>
-      <c r="G4">
-        <v>621</v>
-      </c>
-      <c r="H4">
-        <v>621</v>
-      </c>
-      <c r="J4">
-        <v>621</v>
-      </c>
-      <c r="K4">
-        <v>621</v>
+        <v>589</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C5">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D5">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E5">
-        <v>20</v>
-      </c>
-      <c r="F5">
-        <v>10</v>
-      </c>
-      <c r="G5">
-        <v>20</v>
-      </c>
-      <c r="H5">
-        <v>10</v>
-      </c>
-      <c r="J5">
-        <v>10</v>
-      </c>
-      <c r="K5">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>5.0599999999999999E-2</v>
+        <v>3.1099999999999999E-2</v>
       </c>
       <c r="C6" s="1">
-        <v>3.7199999999999997E-2</v>
+        <v>3.2099999999999997E-2</v>
       </c>
       <c r="D6" s="1">
-        <v>8.6099999999999996E-2</v>
+        <v>2.3599999999999999E-2</v>
       </c>
       <c r="E6" s="1">
-        <v>9.1499999999999998E-2</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0.1019</v>
-      </c>
-      <c r="G6" s="1">
-        <v>9.4500000000000001E-2</v>
-      </c>
-      <c r="H6" s="1">
-        <v>1.7600000000000001E-2</v>
-      </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1">
-        <v>9.8800000000000013E-2</v>
-      </c>
-      <c r="K6" s="1">
-        <v>9.5799999999999996E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2">
-        <f>1-B6</f>
-        <v>0.94940000000000002</v>
-      </c>
-      <c r="C7" s="2">
-        <f t="shared" ref="C7:M7" si="0">1-C6</f>
-        <v>0.96279999999999999</v>
-      </c>
-      <c r="D7" s="2">
-        <f t="shared" si="0"/>
-        <v>0.91390000000000005</v>
-      </c>
-      <c r="E7" s="2">
-        <f t="shared" si="0"/>
-        <v>0.90849999999999997</v>
-      </c>
-      <c r="F7" s="2">
-        <f t="shared" si="0"/>
-        <v>0.89810000000000001</v>
-      </c>
-      <c r="G7" s="2">
-        <f t="shared" si="0"/>
-        <v>0.90549999999999997</v>
-      </c>
-      <c r="H7" s="2">
-        <f t="shared" si="0"/>
-        <v>0.98240000000000005</v>
-      </c>
-      <c r="I7" s="2">
-        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B7" s="1">
+        <f t="shared" ref="B7" si="0">1-B6</f>
+        <v>0.96889999999999998</v>
+      </c>
+      <c r="C7" s="1">
+        <f>1-C6</f>
+        <v>0.96789999999999998</v>
+      </c>
+      <c r="D7" s="1">
+        <f>1-D6</f>
+        <v>0.97640000000000005</v>
+      </c>
+      <c r="E7" s="1">
+        <f>1-E6</f>
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="F7" s="1">
+        <f>1-F6</f>
         <v>1</v>
       </c>
-      <c r="J7" s="2">
-        <f t="shared" si="0"/>
-        <v>0.9012</v>
-      </c>
-      <c r="K7" s="2">
-        <f t="shared" si="0"/>
-        <v>0.9042</v>
-      </c>
-      <c r="L7" s="2">
-        <f t="shared" si="0"/>
+      <c r="G7" s="1">
+        <f>1-G6</f>
         <v>1</v>
       </c>
-      <c r="M7" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
+      <c r="I7" s="2"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B10" s="2">
         <f>B7</f>
-        <v>0.94940000000000002</v>
-      </c>
-      <c r="C10" s="2">
+        <v>0.96889999999999998</v>
+      </c>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="2">
         <f>C7</f>
-        <v>0.96279999999999999</v>
-      </c>
+        <v>0.96789999999999998</v>
+      </c>
+      <c r="C11" s="2"/>
     </row>
-    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="2">
         <f>D7</f>
-        <v>0.91390000000000005</v>
-      </c>
-      <c r="C11" s="2">
+        <v>0.97640000000000005</v>
+      </c>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="2">
         <f>E7</f>
-        <v>0.90849999999999997</v>
+        <v>0.97699999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>128</v>
-      </c>
-      <c r="B12" s="2">
-        <f>F7</f>
-        <v>0.89810000000000001</v>
-      </c>
-      <c r="C12" s="2">
-        <f>G7</f>
-        <v>0.90549999999999997</v>
-      </c>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="2"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="2">
-        <f>H7</f>
-        <v>0.98240000000000005</v>
-      </c>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2">
-        <f>J7</f>
-        <v>0.9012</v>
-      </c>
-      <c r="C14" s="2">
-        <f>K7</f>
-        <v>0.9042</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>13</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B15" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2901,39 +2652,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.42578125" hidden="1" customWidth="1"/>
-    <col min="3" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="7" width="12.42578125" customWidth="1"/>
+    <col min="3" max="8" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="C1">
-        <v>128</v>
+      <c r="C1" t="s">
+        <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
         <v>17</v>
-      </c>
-      <c r="H1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3080,7 +2829,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1">
         <f>AVERAGE(B2:B11)</f>
@@ -3097,7 +2846,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B13" s="4">
         <f>_xlfn.STDEV.P(B2:B11)</f>
@@ -3114,7 +2863,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B14" s="4">
         <f>B13/SQRT(10)</f>

</xml_diff>

<commit_message>
deleted unknown trained models
</commit_message>
<xml_diff>
--- a/Baseline-experimental-results.xlsx
+++ b/Baseline-experimental-results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="new_results" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>Dataset</t>
   </si>
@@ -96,10 +96,7 @@
     <t>128_extended_bin</t>
   </si>
   <si>
-    <t>MEMORY ERROR</t>
-  </si>
-  <si>
-    <t>Extended_augmented</t>
+    <t>Extended_bin_augmented</t>
   </si>
 </sst>
 </file>
@@ -725,10 +722,10 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'10-fold cross validation'!$B$14:$F$14</c:f>
+                <c:f>'10-fold cross validation'!$B$14:$E$14</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="4"/>
+                  <c:ptCount val="3"/>
                   <c:pt idx="0">
                     <c:v>9.8594325187122372E-4</c:v>
                   </c:pt>
@@ -759,9 +756,9 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>'10-fold cross validation'!$B$1:$H$1</c:f>
+              <c:f>'10-fold cross validation'!$B$1:$G$1</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Original</c:v>
                 </c:pt>
@@ -769,26 +766,23 @@
                   <c:v>Original_bin</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Augmented</c:v>
+                  <c:v>Bin_augmented</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Bin_augmented</c:v>
+                  <c:v>Extended_bin</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Extended_bin</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Extended_augmented</c:v>
+                  <c:v>Extended_bin_augmented</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'10-fold cross validation'!$B$12:$H$12</c:f>
+              <c:f>'10-fold cross validation'!$B$12:$G$12</c:f>
               <c:numCache>
                 <c:formatCode>0.0000%</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.968421054</c:v>
                 </c:pt>
@@ -2104,16 +2098,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>14287</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:rowOff>152399</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2440,7 +2434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -2489,9 +2483,6 @@
       <c r="E2">
         <v>196110</v>
       </c>
-      <c r="G2" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -2655,19 +2646,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.42578125" hidden="1" customWidth="1"/>
-    <col min="3" max="8" width="21.5703125" customWidth="1"/>
+    <col min="3" max="7" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -2678,19 +2669,16 @@
         <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2704,9 +2692,8 @@
         <v>0.97034841000000005</v>
       </c>
       <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2720,7 +2707,7 @@
         <v>0.96886583000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2734,7 +2721,7 @@
         <v>0.96738323999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2748,7 +2735,7 @@
         <v>0.97220163000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2762,7 +2749,7 @@
         <v>0.96849518000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2776,7 +2763,7 @@
         <v>0.97405485999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2790,7 +2777,7 @@
         <v>0.96515938000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2804,7 +2791,7 @@
         <v>0.96478872999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2818,7 +2805,7 @@
         <v>0.96960712000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2832,7 +2819,7 @@
         <v>0.96330614999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2849,7 +2836,7 @@
         <v>0.96842105299999992</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2866,7 +2853,7 @@
         <v>3.2004514486180012E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
small changes, need results from 10-fold experiments.
</commit_message>
<xml_diff>
--- a/Baseline-experimental-results.xlsx
+++ b/Baseline-experimental-results.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Dataset</t>
   </si>
@@ -145,7 +145,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -153,6 +153,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Procent" xfId="1" builtinId="5"/>
@@ -722,15 +723,18 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'10-fold cross validation'!$B$14:$E$14</c:f>
+                <c:f>'10-fold cross validation'!$B$14:$F$14</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="3"/>
+                  <c:ptCount val="4"/>
                   <c:pt idx="0">
                     <c:v>9.8594325187122372E-4</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>1.0120716118418233E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2.8765315107973311E-4</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -756,9 +760,9 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>'10-fold cross validation'!$B$1:$G$1</c:f>
+              <c:f>'10-fold cross validation'!$B$1:$H$1</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Original</c:v>
                 </c:pt>
@@ -766,12 +770,15 @@
                   <c:v>Original_bin</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Augmented</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Bin_augmented</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Extended_bin</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Extended_bin_augmented</c:v>
                 </c:pt>
               </c:strCache>
@@ -779,15 +786,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'10-fold cross validation'!$B$12:$G$12</c:f>
+              <c:f>'10-fold cross validation'!$B$12:$H$12</c:f>
               <c:numCache>
                 <c:formatCode>0.0000%</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0.968421054</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.96842105299999992</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.97658385299999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2104,7 +2114,7 @@
       <xdr:rowOff>28574</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>314325</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>152399</xdr:rowOff>
@@ -2646,19 +2656,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.42578125" hidden="1" customWidth="1"/>
-    <col min="3" max="7" width="21.5703125" customWidth="1"/>
+    <col min="3" max="8" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -2669,16 +2679,19 @@
         <v>15</v>
       </c>
       <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2692,8 +2705,11 @@
         <v>0.97034841000000005</v>
       </c>
       <c r="E2" s="5"/>
+      <c r="F2" s="4">
+        <v>0.97531922000000004</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2706,8 +2722,12 @@
       <c r="D3" s="5">
         <v>0.96886583000000004</v>
       </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="7">
+        <v>0.97654306000000002</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2720,8 +2740,12 @@
       <c r="D4" s="5">
         <v>0.96738323999999998</v>
       </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="7">
+        <v>0.97678783000000002</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2734,8 +2758,12 @@
       <c r="D5" s="5">
         <v>0.97220163000000004</v>
       </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="7">
+        <v>0.97580875</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2748,8 +2776,12 @@
       <c r="D6" s="5">
         <v>0.96849518000000001</v>
       </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="7">
+        <v>0.97784848999999996</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2762,8 +2794,12 @@
       <c r="D7" s="5">
         <v>0.97405485999999997</v>
       </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="7">
+        <v>0.97560477999999995</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2776,8 +2812,12 @@
       <c r="D8" s="5">
         <v>0.96515938000000001</v>
       </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="7">
+        <v>0.97703260000000003</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2790,8 +2830,12 @@
       <c r="D9" s="5">
         <v>0.96478872999999998</v>
       </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="7">
+        <v>0.97833802000000003</v>
+      </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2804,8 +2848,12 @@
       <c r="D10" s="5">
         <v>0.96960712000000004</v>
       </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="7">
+        <v>0.97621670000000005</v>
+      </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2818,8 +2866,12 @@
       <c r="D11" s="5">
         <v>0.96330614999999997</v>
       </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="7">
+        <v>0.97633908000000003</v>
+      </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2835,8 +2887,13 @@
         <f>AVERAGE(D2:D11)</f>
         <v>0.96842105299999992</v>
       </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6">
+        <f>AVERAGE(F2:F11)</f>
+        <v>0.97658385299999995</v>
+      </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2852,8 +2909,13 @@
         <f>_xlfn.STDEV.P(D2:D11)</f>
         <v>3.2004514486180012E-3</v>
       </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4">
+        <f>_xlfn.STDEV.P(F2:F11)</f>
+        <v>9.0963913353647979E-4</v>
+      </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -2868,6 +2930,11 @@
       <c r="D14" s="4">
         <f>D13/SQRT(10)</f>
         <v>1.0120716118418233E-3</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4">
+        <f>F13/SQRT(10)</f>
+        <v>2.8765315107973311E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rogiers files for the day
</commit_message>
<xml_diff>
--- a/Baseline-experimental-results.xlsx
+++ b/Baseline-experimental-results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="new_results" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>Dataset</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>128_over_99</t>
-  </si>
-  <si>
-    <t>128_times_10</t>
   </si>
   <si>
     <t>classes</t>
@@ -75,22 +72,13 @@
     <t>Original_bin</t>
   </si>
   <si>
-    <t>Extended</t>
-  </si>
-  <si>
     <t>Extended_bin</t>
-  </si>
-  <si>
-    <t>Augmented</t>
   </si>
   <si>
     <t>Bin_augmented</t>
   </si>
   <si>
     <t>Bin_Augmented</t>
-  </si>
-  <si>
-    <t>128_extended</t>
   </si>
   <si>
     <t>128_extended_bin</t>
@@ -117,16 +105,16 @@
     <t>DCNN</t>
   </si>
   <si>
-    <t>1NN</t>
-  </si>
-  <si>
     <t>No_dropout</t>
   </si>
   <si>
     <t>Orig_Bin_No_Dropout</t>
   </si>
   <si>
-    <t>Baseline_train_128_extended_bin</t>
+    <t>MLP</t>
+  </si>
+  <si>
+    <t>CNN</t>
   </si>
 </sst>
 </file>
@@ -218,36 +206,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -264,7 +222,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Accuracy</c:v>
+                  <c:v>MLP</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -339,25 +297,16 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>new_results!$A$10:$A$15</c:f>
+              <c:f>new_results!$A$10:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Original</c:v>
+                  <c:v>Original_bin</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Original_bin</c:v>
+                  <c:v>Bin_Augmented</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Augmented</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Bin_Augmented</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Extended</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>Extended_bin</c:v>
                 </c:pt>
               </c:strCache>
@@ -365,20 +314,128 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>new_results!$B$10:$B$15</c:f>
+              <c:f>new_results!$B$10:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-59AE-4932-B23F-6456F083D2FC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>new_results!$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CNN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="nl-NL"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>new_results!$A$10:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Original_bin</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bin_Augmented</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Extended_bin</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>new_results!$C$10:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.96889999999999998</c:v>
+                  <c:v>0.96789999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.96789999999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.97640000000000005</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>0.97699999999999998</c:v>
                 </c:pt>
               </c:numCache>
@@ -386,7 +443,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-59AE-4932-B23F-6456F083D2FC}"/>
+              <c16:uniqueId val="{00000000-2A99-4E4C-A4D6-42531CE76C50}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -478,7 +535,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2050,13 +2107,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1033462</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>957262</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2423,10 +2480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2439,23 +2496,14 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>128</v>
+      <c r="B1" t="s">
+        <v>8</v>
       </c>
       <c r="C1" t="s">
         <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2466,12 +2514,6 @@
         <v>21584</v>
       </c>
       <c r="C2">
-        <v>21584</v>
-      </c>
-      <c r="D2">
-        <v>196180</v>
-      </c>
-      <c r="E2">
         <v>196110</v>
       </c>
     </row>
@@ -2483,29 +2525,17 @@
         <v>5396</v>
       </c>
       <c r="C3">
-        <v>5396</v>
-      </c>
-      <c r="D3">
-        <v>49045</v>
-      </c>
-      <c r="E3">
         <v>49027</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>589</v>
       </c>
       <c r="C4">
-        <v>589</v>
-      </c>
-      <c r="D4">
-        <v>589</v>
-      </c>
-      <c r="E4">
         <v>589</v>
       </c>
     </row>
@@ -2519,115 +2549,68 @@
       <c r="C5">
         <v>4</v>
       </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
-      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>3.1099999999999999E-2</v>
+        <v>3.2099999999999997E-2</v>
       </c>
       <c r="C6" s="1">
-        <v>3.2099999999999997E-2</v>
-      </c>
-      <c r="D6" s="1">
-        <v>2.3599999999999999E-2</v>
-      </c>
-      <c r="E6" s="1">
         <v>2.3E-2</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1">
-        <f t="shared" ref="B7" si="0">1-B6</f>
-        <v>0.96889999999999998</v>
+        <f>1-B6</f>
+        <v>0.96789999999999998</v>
       </c>
       <c r="C7" s="1">
         <f>1-C6</f>
-        <v>0.96789999999999998</v>
+        <v>0.97699999999999998</v>
       </c>
       <c r="D7" s="1">
         <f>1-D6</f>
-        <v>0.97640000000000005</v>
-      </c>
-      <c r="E7" s="1">
-        <f>1-E6</f>
-        <v>0.97699999999999998</v>
-      </c>
-      <c r="F7" s="1">
-        <f>1-F6</f>
         <v>1</v>
       </c>
-      <c r="G7" s="1">
-        <f>1-G6</f>
-        <v>1</v>
-      </c>
+      <c r="F7" s="1"/>
       <c r="I7" s="2"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>8</v>
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="2">
+      <c r="C10" s="2">
         <f>B7</f>
-        <v>0.96889999999999998</v>
-      </c>
-      <c r="C10" s="2"/>
+        <v>0.96789999999999998</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="2">
+        <v>17</v>
+      </c>
+      <c r="C11" s="2">
         <f>C7</f>
-        <v>0.96789999999999998</v>
-      </c>
-      <c r="C11" s="2"/>
+        <v>0.97699999999999998</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="2">
-        <f>D7</f>
-        <v>0.97640000000000005</v>
+        <v>15</v>
       </c>
       <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="2">
-        <f>E7</f>
-        <v>0.97699999999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2639,8 +2622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N36" sqref="N36"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2658,25 +2641,22 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>19</v>
-      </c>
-      <c r="G1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2701,9 +2681,7 @@
       <c r="G2" s="4">
         <v>0.99415492999999999</v>
       </c>
-      <c r="K2" s="4">
-        <v>0.99231272999999998</v>
-      </c>
+      <c r="K2" s="4"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -2914,7 +2892,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1">
         <f>AVERAGE(B2:B11)</f>
@@ -2947,40 +2925,40 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="4">
-        <f>_xlfn.STDEV.P(B2:B11)</f>
+        <f t="shared" ref="B13:G13" si="1">_xlfn.STDEV.P(B2:B11)</f>
         <v>4.864772519873984E-3</v>
       </c>
       <c r="C13" s="4">
-        <f>_xlfn.STDEV.P(C2:C11)</f>
+        <f t="shared" si="1"/>
         <v>3.1178263195861368E-3</v>
       </c>
       <c r="D13" s="4">
-        <f>_xlfn.STDEV.P(D2:D11)</f>
+        <f t="shared" si="1"/>
         <v>3.2004514486180012E-3</v>
       </c>
       <c r="E13" s="4">
-        <f>_xlfn.STDEV.P(E2:E11)</f>
+        <f t="shared" si="1"/>
         <v>3.375923455316478E-3</v>
       </c>
       <c r="F13" s="4">
-        <f>_xlfn.STDEV.P(F2:F11)</f>
+        <f t="shared" si="1"/>
         <v>9.0963913353647979E-4</v>
       </c>
       <c r="G13" s="4">
-        <f>_xlfn.STDEV.P(G2:G11)</f>
+        <f t="shared" si="1"/>
         <v>3.9392551964172325E-4</v>
       </c>
       <c r="H13" s="4" t="e">
-        <f t="shared" ref="G13:H13" si="1">_xlfn.STDEV.P(H2:H11)</f>
+        <f t="shared" ref="H13" si="2">_xlfn.STDEV.P(H2:H11)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="4">
         <f>B13/SQRT(10)</f>
@@ -3003,32 +2981,30 @@
         <v>2.8765315107973311E-4</v>
       </c>
       <c r="G14" s="4">
-        <f t="shared" ref="G14:H14" si="2">G13/SQRT(10)</f>
+        <f t="shared" ref="G14:H14" si="3">G13/SQRT(10)</f>
         <v>1.2457018705332415E-4</v>
       </c>
       <c r="H14" s="4" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D17" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="9">
-        <v>0.85</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="C18" s="9"/>
       <c r="D18" s="8">
         <f>C$12</f>
         <v>0.968421054</v>
@@ -3036,11 +3012,9 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="9">
-        <v>0</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C19" s="9"/>
       <c r="D19" s="8">
         <f>D$12</f>
         <v>0.96842105299999992</v>
@@ -3048,7 +3022,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D20" s="8">
         <f>E12</f>
@@ -3057,11 +3031,9 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="9">
-        <v>0</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="C21" s="9"/>
       <c r="D21" s="8">
         <f>F12</f>
         <v>0.97658385299999995</v>
@@ -3069,11 +3041,9 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="9">
-        <v>0</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="C22" s="9"/>
       <c r="D22" s="8">
         <f>G12</f>
         <v>0.99395070499999993</v>
@@ -3081,11 +3051,9 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="9">
-        <v>0</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C23" s="9"/>
       <c r="D23" s="8" t="e">
         <f>H12</f>
         <v>#DIV/0!</v>

</xml_diff>